<commit_message>
Segundo commit: adicionando arquivos do projeto Xperiun
</commit_message>
<xml_diff>
--- a/Documentacao Squad 10 - Data Challenge 01 - Medidas e Premissas.xlsx
+++ b/Documentacao Squad 10 - Data Challenge 01 - Medidas e Premissas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5919c369ad4368/portifolio/Moduloprodutivo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8D65936E-1BF4-476F-BCE7-F8AD7DECBBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAEE756C-4373-43B8-92D2-0696389D2569}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8D65936E-1BF4-476F-BCE7-F8AD7DECBBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE919E68-6F9C-4784-B84A-CE6D7332A035}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1477,7 +1477,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1604,9 +1604,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1644,7 +1644,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1750,7 +1750,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1892,7 +1892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1903,24 +1903,24 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="C3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" style="10" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="3" customWidth="1"/>
-    <col min="9" max="10" width="26.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" style="10" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="26.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="72">
+    <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="144">
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="106.5">
+    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="72">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="144">
+    <row r="6" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="57.6">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.45">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29.45">
+    <row r="9" spans="1:10" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29.45">
+    <row r="10" spans="1:10" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.15">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="129.6">
+    <row r="14" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="100.9">
+    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.9">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="129.6">
+    <row r="17" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="57.6">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>10</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="43.15">
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="115.15">
+    <row r="20" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="72">
+    <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="86.45">
+    <row r="22" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="43.15">
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="29.45">
+    <row r="24" spans="1:9" ht="29.4" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="43.15">
+    <row r="25" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>10</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="28.9">
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>10</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>10</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="72">
+    <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="57.6">
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>10</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28.9">
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.6">
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="57.6">
+    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>10</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="172.9">
+    <row r="33" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>10</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="129.6">
+    <row r="34" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="115.15">
+    <row r="35" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>10</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="100.9">
+    <row r="36" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>10</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="115.15">
+    <row r="37" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>10</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="115.15">
+    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="28.9">
+    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>10</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="115.15">
+    <row r="40" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>10</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="28.9">
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>10</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="115.15">
+    <row r="42" spans="1:9" ht="115.2" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>10</v>
       </c>
@@ -3118,6 +3118,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="8HJzbNEzJGP+RSlSZsK6ENSRMXrPTkIWK+EZx7Q+oy5pBilx/FyviQrmGV8RDrhGRq068GcTWlT+jE0fl63hfQ==" saltValue="4E+sBBGNfhXA0putTZW/GQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" pivotTables="0"/>
   <autoFilter ref="A1:J42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3132,9 +3133,9 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>225</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>225</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>225</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>225</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>225</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>225</v>
       </c>
@@ -3286,7 +3287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>225</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>225</v>
       </c>
@@ -3345,7 +3346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>225</v>
       </c>
@@ -3359,7 +3360,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>225</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>243</v>
       </c>
@@ -3387,7 +3388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>243</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>243</v>
       </c>
@@ -3415,7 +3416,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>243</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>248</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>248</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>248</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>248</v>
       </c>
@@ -3499,7 +3500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>248</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>248</v>
       </c>
@@ -3527,7 +3528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>248</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>248</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>248</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>248</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>248</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>248</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>248</v>
       </c>
@@ -3625,7 +3626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>248</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>248</v>
       </c>
@@ -3653,7 +3654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>265</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>265</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>265</v>
       </c>
@@ -3695,7 +3696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>265</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>265</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>265</v>
       </c>
@@ -3737,7 +3738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>265</v>
       </c>
@@ -3751,7 +3752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>265</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>265</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>276</v>
       </c>
@@ -3793,7 +3794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>276</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>276</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -3835,7 +3836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>276</v>
       </c>
@@ -3849,7 +3850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>276</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>276</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>284</v>
       </c>
@@ -3891,7 +3892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>284</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>284</v>
       </c>
@@ -3919,7 +3920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>284</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>284</v>
       </c>
@@ -3947,7 +3948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>284</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>284</v>
       </c>
@@ -3975,7 +3976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>284</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>284</v>
       </c>
@@ -4003,7 +4004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>284</v>
       </c>
@@ -4017,7 +4018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>284</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>284</v>
       </c>
@@ -4045,7 +4046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>284</v>
       </c>
@@ -4059,7 +4060,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>284</v>
       </c>
@@ -4073,7 +4074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>284</v>
       </c>
@@ -4087,7 +4088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>296</v>
       </c>
@@ -4101,7 +4102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>296</v>
       </c>
@@ -4115,7 +4116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>296</v>
       </c>
@@ -4129,7 +4130,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>296</v>
       </c>
@@ -4143,7 +4144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>296</v>
       </c>
@@ -4157,7 +4158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>296</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>296</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>296</v>
       </c>
@@ -4199,7 +4200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>296</v>
       </c>
@@ -4213,7 +4214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>296</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>296</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>296</v>
       </c>
@@ -4255,7 +4256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>296</v>
       </c>
@@ -4269,7 +4270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>296</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>296</v>
       </c>
@@ -4297,7 +4298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>296</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>296</v>
       </c>
@@ -4325,7 +4326,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>296</v>
       </c>
@@ -4339,7 +4340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>296</v>
       </c>
@@ -4353,7 +4354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>296</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>296</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>296</v>
       </c>
@@ -4395,7 +4396,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>296</v>
       </c>
@@ -4424,9 +4425,9 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>317</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>39</v>
       </c>
@@ -4502,7 +4503,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>44</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>45</v>
       </c>
@@ -4616,7 +4617,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>47</v>
       </c>
@@ -4654,7 +4655,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>35</v>
       </c>
@@ -4692,7 +4693,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>37</v>
       </c>
@@ -4730,7 +4731,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>38</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>42</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>41</v>
       </c>
@@ -4844,7 +4845,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>43</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>34</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>36</v>
       </c>
@@ -4958,7 +4959,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>46</v>
       </c>
@@ -5011,9 +5012,9 @@
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -5021,7 +5022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>366</v>
       </c>
@@ -5047,12 +5048,12 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>368</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="302.45">
+    <row r="2" spans="1:7" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -5095,7 +5096,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.6">
+    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>13</v>
       </c>
@@ -5115,7 +5116,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="409.6">
+    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -5135,7 +5136,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="409.6">
+    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>19</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="409.6">
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>22</v>
       </c>
@@ -5175,7 +5176,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.6">
+    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="409.6">
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>28</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="216">
+    <row r="9" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>31</v>
       </c>

</xml_diff>